<commit_message>
feat: integrate logo into report
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ryanrent.sharepoint.com/sites/RyanRent/Gedeelde documenten/General/01_RyanRent&amp;Co/Aljereau/Eindafrekening Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_F51AB12D18F85E02B57FD3F3AEC58B057A3FE71A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41C012F5-6B0D-1E4E-BD2A-7B14FB9FA91F}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F51AB12D18F85E02B57FD3F3AEC58B057A3FE71A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692778C7-7F23-1043-9260-3E5563684049}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,20 @@
     <sheet name="Hoofdgegevens" sheetId="1" r:id="rId1"/>
     <sheet name="Schades Detail" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -468,7 +481,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -556,7 +569,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>350</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +577,8 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>450</v>
+        <f>SUM(B15:B17)</f>
+        <v>10001275</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +594,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -588,7 +602,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>